<commit_message>
Added iterations for measuretime
</commit_message>
<xml_diff>
--- a/graphics/algorithm_times.xlsx
+++ b/graphics/algorithm_times.xlsx
@@ -443,10 +443,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5.3e-06</v>
+        <v>0.0467633</v>
       </c>
       <c r="C2" t="n">
-        <v>4.4e-06</v>
+        <v>0.0487335</v>
       </c>
     </row>
     <row r="3">
@@ -454,10 +454,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>0.008133899999999999</v>
+        <v>0.07045319999999999</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0051576</v>
+        <v>0.06695479999999999</v>
       </c>
     </row>
     <row r="4">
@@ -465,10 +465,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0134836</v>
+        <v>0.06944699999999999</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0092493</v>
+        <v>0.073643</v>
       </c>
     </row>
     <row r="5">
@@ -476,10 +476,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>0.018345</v>
+        <v>0.0687446</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0136249</v>
+        <v>0.0684003</v>
       </c>
     </row>
     <row r="6">
@@ -487,10 +487,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0232282</v>
+        <v>0.07184649999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0180628</v>
+        <v>0.0763292</v>
       </c>
     </row>
     <row r="7">
@@ -498,10 +498,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>0.029644</v>
+        <v>0.0677532</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0228163</v>
+        <v>0.0765948</v>
       </c>
     </row>
     <row r="8">
@@ -509,10 +509,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>0.035297</v>
+        <v>0.06634710000000001</v>
       </c>
       <c r="C8" t="n">
-        <v>0.02703</v>
+        <v>0.07066119999999999</v>
       </c>
     </row>
     <row r="9">
@@ -520,10 +520,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0407023</v>
+        <v>0.06604549999999999</v>
       </c>
       <c r="C9" t="n">
-        <v>0.031822</v>
+        <v>0.0701191</v>
       </c>
     </row>
     <row r="10">
@@ -531,10 +531,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>0.047122</v>
+        <v>0.0651026</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0359244</v>
+        <v>0.0713932</v>
       </c>
     </row>
     <row r="11">
@@ -542,10 +542,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0525468</v>
+        <v>0.06485009999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0410559</v>
+        <v>0.0757284</v>
       </c>
     </row>
     <row r="12">
@@ -553,10 +553,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0599231</v>
+        <v>0.06514739999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0514031</v>
+        <v>0.0735261</v>
       </c>
     </row>
     <row r="13">
@@ -564,10 +564,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0633946</v>
+        <v>0.0643561</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0503434</v>
+        <v>0.0734255</v>
       </c>
     </row>
     <row r="14">
@@ -575,10 +575,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>0.0690693</v>
+        <v>0.06486889999999999</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0535569</v>
+        <v>0.0746039</v>
       </c>
     </row>
     <row r="15">
@@ -586,10 +586,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>0.0760178</v>
+        <v>0.06350889999999999</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0580229</v>
+        <v>0.07324840000000001</v>
       </c>
     </row>
     <row r="16">
@@ -597,10 +597,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>0.08719449999999999</v>
+        <v>0.06327149999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>0.06376560000000001</v>
+        <v>0.07385799999999999</v>
       </c>
     </row>
     <row r="17">
@@ -608,10 +608,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0908952</v>
+        <v>0.0625245</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0705017</v>
+        <v>0.07481309999999999</v>
       </c>
     </row>
     <row r="18">
@@ -619,10 +619,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>0.0969981</v>
+        <v>0.0614723</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0749599</v>
+        <v>0.0752569</v>
       </c>
     </row>
     <row r="19">
@@ -630,10 +630,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>0.109144</v>
+        <v>0.0613532</v>
       </c>
       <c r="C19" t="n">
-        <v>0.08128489999999999</v>
+        <v>0.0757472</v>
       </c>
     </row>
     <row r="20">
@@ -641,10 +641,10 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>0.106829</v>
+        <v>0.0616428</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0804424</v>
+        <v>0.07676769999999999</v>
       </c>
     </row>
     <row r="21">
@@ -652,10 +652,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>0.111731</v>
+        <v>0.0639245</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0855876</v>
+        <v>0.077359</v>
       </c>
     </row>
     <row r="22">
@@ -663,10 +663,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>0.116777</v>
+        <v>0.0624081</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0897271</v>
+        <v>0.07936559999999999</v>
       </c>
     </row>
     <row r="23">
@@ -674,10 +674,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>0.125623</v>
+        <v>0.0597885</v>
       </c>
       <c r="C23" t="n">
-        <v>0.09352389999999999</v>
+        <v>0.079052</v>
       </c>
     </row>
     <row r="24">
@@ -685,10 +685,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>0.127859</v>
+        <v>0.0584506</v>
       </c>
       <c r="C24" t="n">
-        <v>0.103191</v>
+        <v>0.0815068</v>
       </c>
     </row>
     <row r="25">
@@ -696,10 +696,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>0.138649</v>
+        <v>0.062557</v>
       </c>
       <c r="C25" t="n">
-        <v>0.104463</v>
+        <v>0.0803644</v>
       </c>
     </row>
     <row r="26">
@@ -707,10 +707,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>0.139258</v>
+        <v>0.0642065</v>
       </c>
       <c r="C26" t="n">
-        <v>0.107633</v>
+        <v>0.08063380000000001</v>
       </c>
     </row>
     <row r="27">
@@ -718,10 +718,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>0.147782</v>
+        <v>0.0566824</v>
       </c>
       <c r="C27" t="n">
-        <v>0.11305</v>
+        <v>0.0796277</v>
       </c>
     </row>
     <row r="28">
@@ -729,10 +729,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>0.155463</v>
+        <v>0.0569589</v>
       </c>
       <c r="C28" t="n">
-        <v>0.122654</v>
+        <v>0.0804494</v>
       </c>
     </row>
     <row r="29">
@@ -740,10 +740,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>0.159298</v>
+        <v>0.0556992</v>
       </c>
       <c r="C29" t="n">
-        <v>0.1211</v>
+        <v>0.08298659999999999</v>
       </c>
     </row>
     <row r="30">
@@ -751,10 +751,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>0.162387</v>
+        <v>0.0549723</v>
       </c>
       <c r="C30" t="n">
-        <v>0.129245</v>
+        <v>0.08191229999999999</v>
       </c>
     </row>
     <row r="31">
@@ -762,10 +762,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>0.168407</v>
+        <v>0.0544828</v>
       </c>
       <c r="C31" t="n">
-        <v>0.129919</v>
+        <v>0.0835911</v>
       </c>
     </row>
     <row r="32">
@@ -773,10 +773,10 @@
         <v>31</v>
       </c>
       <c r="B32" t="n">
-        <v>0.176378</v>
+        <v>0.0549093</v>
       </c>
       <c r="C32" t="n">
-        <v>0.137409</v>
+        <v>0.0839536</v>
       </c>
     </row>
     <row r="33">
@@ -784,10 +784,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="n">
-        <v>0.179471</v>
+        <v>0.0535964</v>
       </c>
       <c r="C33" t="n">
-        <v>0.141274</v>
+        <v>0.0850148</v>
       </c>
     </row>
     <row r="34">
@@ -795,10 +795,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="n">
-        <v>0.191988</v>
+        <v>0.0537806</v>
       </c>
       <c r="C34" t="n">
-        <v>0.143494</v>
+        <v>0.0836634</v>
       </c>
     </row>
     <row r="35">
@@ -806,10 +806,10 @@
         <v>34</v>
       </c>
       <c r="B35" t="n">
-        <v>0.191613</v>
+        <v>0.0540613</v>
       </c>
       <c r="C35" t="n">
-        <v>0.148226</v>
+        <v>0.08407050000000001</v>
       </c>
     </row>
     <row r="36">
@@ -817,10 +817,10 @@
         <v>35</v>
       </c>
       <c r="B36" t="n">
-        <v>0.1965</v>
+        <v>0.0535874</v>
       </c>
       <c r="C36" t="n">
-        <v>0.15837</v>
+        <v>0.08498219999999999</v>
       </c>
     </row>
     <row r="37">
@@ -828,10 +828,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="n">
-        <v>0.2082</v>
+        <v>0.0522843</v>
       </c>
       <c r="C37" t="n">
-        <v>0.160752</v>
+        <v>0.0859414</v>
       </c>
     </row>
     <row r="38">
@@ -839,10 +839,10 @@
         <v>37</v>
       </c>
       <c r="B38" t="n">
-        <v>0.208949</v>
+        <v>0.0519608</v>
       </c>
       <c r="C38" t="n">
-        <v>0.160888</v>
+        <v>0.0864109</v>
       </c>
     </row>
     <row r="39">
@@ -850,10 +850,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="n">
-        <v>0.215054</v>
+        <v>0.050965</v>
       </c>
       <c r="C39" t="n">
-        <v>0.16736</v>
+        <v>0.0864138</v>
       </c>
     </row>
     <row r="40">
@@ -861,10 +861,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="n">
-        <v>0.231881</v>
+        <v>0.0508956</v>
       </c>
       <c r="C40" t="n">
-        <v>0.174486</v>
+        <v>0.08933720000000001</v>
       </c>
     </row>
     <row r="41">
@@ -872,10 +872,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="n">
-        <v>0.233503</v>
+        <v>0.0534747</v>
       </c>
       <c r="C41" t="n">
-        <v>0.179867</v>
+        <v>0.08889619999999999</v>
       </c>
     </row>
     <row r="42">
@@ -883,10 +883,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="n">
-        <v>0.231188</v>
+        <v>0.0684694</v>
       </c>
       <c r="C42" t="n">
-        <v>0.187319</v>
+        <v>0.0975973</v>
       </c>
     </row>
     <row r="43">
@@ -894,10 +894,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>0.241309</v>
+        <v>0.0504215</v>
       </c>
       <c r="C43" t="n">
-        <v>0.185078</v>
+        <v>0.0925718</v>
       </c>
     </row>
     <row r="44">
@@ -905,10 +905,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="n">
-        <v>0.24773</v>
+        <v>0.0493211</v>
       </c>
       <c r="C44" t="n">
-        <v>0.192259</v>
+        <v>0.09393899999999999</v>
       </c>
     </row>
     <row r="45">
@@ -916,10 +916,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="n">
-        <v>0.251351</v>
+        <v>0.0481868</v>
       </c>
       <c r="C45" t="n">
-        <v>0.201894</v>
+        <v>0.09102789999999999</v>
       </c>
     </row>
     <row r="46">
@@ -927,10 +927,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="n">
-        <v>0.254098</v>
+        <v>0.0476639</v>
       </c>
       <c r="C46" t="n">
-        <v>0.199159</v>
+        <v>0.0913003</v>
       </c>
     </row>
     <row r="47">
@@ -938,10 +938,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="n">
-        <v>0.277607</v>
+        <v>0.0497213</v>
       </c>
       <c r="C47" t="n">
-        <v>0.202091</v>
+        <v>0.0909706</v>
       </c>
     </row>
     <row r="48">
@@ -949,10 +949,10 @@
         <v>47</v>
       </c>
       <c r="B48" t="n">
-        <v>0.265178</v>
+        <v>0.0460525</v>
       </c>
       <c r="C48" t="n">
-        <v>0.216191</v>
+        <v>0.0980834</v>
       </c>
     </row>
     <row r="49">
@@ -960,10 +960,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="n">
-        <v>0.274966</v>
+        <v>0.0501845</v>
       </c>
       <c r="C49" t="n">
-        <v>0.215527</v>
+        <v>0.0922331</v>
       </c>
     </row>
     <row r="50">
@@ -971,10 +971,10 @@
         <v>49</v>
       </c>
       <c r="B50" t="n">
-        <v>0.281608</v>
+        <v>0.0455816</v>
       </c>
       <c r="C50" t="n">
-        <v>0.216887</v>
+        <v>0.09217500000000001</v>
       </c>
     </row>
     <row r="51">
@@ -982,10 +982,10 @@
         <v>50</v>
       </c>
       <c r="B51" t="n">
-        <v>0.286973</v>
+        <v>0.0459533</v>
       </c>
       <c r="C51" t="n">
-        <v>0.226861</v>
+        <v>0.0967678</v>
       </c>
     </row>
     <row r="52">
@@ -993,10 +993,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="n">
-        <v>0.29265</v>
+        <v>0.0442078</v>
       </c>
       <c r="C52" t="n">
-        <v>0.224745</v>
+        <v>0.0943138</v>
       </c>
     </row>
     <row r="53">
@@ -1004,10 +1004,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="n">
-        <v>0.299289</v>
+        <v>0.0459689</v>
       </c>
       <c r="C53" t="n">
-        <v>0.233215</v>
+        <v>0.09400650000000001</v>
       </c>
     </row>
     <row r="54">
@@ -1015,10 +1015,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="n">
-        <v>0.306667</v>
+        <v>0.0435796</v>
       </c>
       <c r="C54" t="n">
-        <v>0.236783</v>
+        <v>0.0962325</v>
       </c>
     </row>
     <row r="55">
@@ -1026,10 +1026,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="n">
-        <v>0.307695</v>
+        <v>0.043721</v>
       </c>
       <c r="C55" t="n">
-        <v>0.241632</v>
+        <v>0.0948382</v>
       </c>
     </row>
     <row r="56">
@@ -1037,10 +1037,10 @@
         <v>55</v>
       </c>
       <c r="B56" t="n">
-        <v>0.320137</v>
+        <v>0.0428141</v>
       </c>
       <c r="C56" t="n">
-        <v>0.247221</v>
+        <v>0.09578979999999999</v>
       </c>
     </row>
     <row r="57">
@@ -1048,10 +1048,10 @@
         <v>56</v>
       </c>
       <c r="B57" t="n">
-        <v>0.32591</v>
+        <v>0.0420995</v>
       </c>
       <c r="C57" t="n">
-        <v>0.251608</v>
+        <v>0.100265</v>
       </c>
     </row>
     <row r="58">
@@ -1059,10 +1059,10 @@
         <v>57</v>
       </c>
       <c r="B58" t="n">
-        <v>0.323052</v>
+        <v>0.0419807</v>
       </c>
       <c r="C58" t="n">
-        <v>0.259739</v>
+        <v>0.0973691</v>
       </c>
     </row>
     <row r="59">
@@ -1070,10 +1070,10 @@
         <v>58</v>
       </c>
       <c r="B59" t="n">
-        <v>0.330242</v>
+        <v>0.0417504</v>
       </c>
       <c r="C59" t="n">
-        <v>0.25711</v>
+        <v>0.0975861</v>
       </c>
     </row>
     <row r="60">
@@ -1081,10 +1081,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="n">
-        <v>0.339025</v>
+        <v>0.0416881</v>
       </c>
       <c r="C60" t="n">
-        <v>0.265909</v>
+        <v>0.09812800000000001</v>
       </c>
     </row>
     <row r="61">
@@ -1092,10 +1092,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="n">
-        <v>0.345518</v>
+        <v>0.0403392</v>
       </c>
       <c r="C61" t="n">
-        <v>0.267064</v>
+        <v>0.0991388</v>
       </c>
     </row>
     <row r="62">
@@ -1103,10 +1103,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="n">
-        <v>0.350502</v>
+        <v>0.039616</v>
       </c>
       <c r="C62" t="n">
-        <v>0.269831</v>
+        <v>0.0999492</v>
       </c>
     </row>
     <row r="63">
@@ -1114,10 +1114,10 @@
         <v>62</v>
       </c>
       <c r="B63" t="n">
-        <v>0.355444</v>
+        <v>0.0389807</v>
       </c>
       <c r="C63" t="n">
-        <v>0.275397</v>
+        <v>0.103598</v>
       </c>
     </row>
     <row r="64">
@@ -1125,10 +1125,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="n">
-        <v>0.363317</v>
+        <v>0.0386416</v>
       </c>
       <c r="C64" t="n">
-        <v>0.282911</v>
+        <v>0.100801</v>
       </c>
     </row>
     <row r="65">
@@ -1136,10 +1136,10 @@
         <v>64</v>
       </c>
       <c r="B65" t="n">
-        <v>0.37003</v>
+        <v>0.0407718</v>
       </c>
       <c r="C65" t="n">
-        <v>0.284026</v>
+        <v>0.101056</v>
       </c>
     </row>
     <row r="66">
@@ -1147,10 +1147,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="n">
-        <v>0.379142</v>
+        <v>0.0374552</v>
       </c>
       <c r="C66" t="n">
-        <v>0.293828</v>
+        <v>0.101664</v>
       </c>
     </row>
     <row r="67">
@@ -1158,10 +1158,10 @@
         <v>66</v>
       </c>
       <c r="B67" t="n">
-        <v>0.378581</v>
+        <v>0.0367964</v>
       </c>
       <c r="C67" t="n">
-        <v>0.291558</v>
+        <v>0.101588</v>
       </c>
     </row>
     <row r="68">
@@ -1169,10 +1169,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="n">
-        <v>0.384419</v>
+        <v>0.0366471</v>
       </c>
       <c r="C68" t="n">
-        <v>0.298276</v>
+        <v>0.102827</v>
       </c>
     </row>
     <row r="69">
@@ -1180,10 +1180,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="n">
-        <v>0.387002</v>
+        <v>0.035756</v>
       </c>
       <c r="C69" t="n">
-        <v>0.302072</v>
+        <v>0.105723</v>
       </c>
     </row>
     <row r="70">
@@ -1191,10 +1191,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="n">
-        <v>0.398043</v>
+        <v>0.0358421</v>
       </c>
       <c r="C70" t="n">
-        <v>0.306297</v>
+        <v>0.104518</v>
       </c>
     </row>
     <row r="71">
@@ -1202,10 +1202,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="n">
-        <v>0.398707</v>
+        <v>0.0361845</v>
       </c>
       <c r="C71" t="n">
-        <v>0.318802</v>
+        <v>0.103434</v>
       </c>
     </row>
     <row r="72">
@@ -1213,10 +1213,10 @@
         <v>71</v>
       </c>
       <c r="B72" t="n">
-        <v>0.410512</v>
+        <v>0.0341179</v>
       </c>
       <c r="C72" t="n">
-        <v>0.318637</v>
+        <v>0.105703</v>
       </c>
     </row>
     <row r="73">
@@ -1224,10 +1224,10 @@
         <v>72</v>
       </c>
       <c r="B73" t="n">
-        <v>0.41728</v>
+        <v>0.0335061</v>
       </c>
       <c r="C73" t="n">
-        <v>0.330544</v>
+        <v>0.104974</v>
       </c>
     </row>
     <row r="74">
@@ -1235,10 +1235,10 @@
         <v>73</v>
       </c>
       <c r="B74" t="n">
-        <v>0.423186</v>
+        <v>0.0352373</v>
       </c>
       <c r="C74" t="n">
-        <v>0.323416</v>
+        <v>0.111499</v>
       </c>
     </row>
     <row r="75">
@@ -1246,10 +1246,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="n">
-        <v>0.422039</v>
+        <v>0.0329565</v>
       </c>
       <c r="C75" t="n">
-        <v>0.328197</v>
+        <v>0.11336</v>
       </c>
     </row>
     <row r="76">
@@ -1257,10 +1257,10 @@
         <v>75</v>
       </c>
       <c r="B76" t="n">
-        <v>0.431266</v>
+        <v>0.0332007</v>
       </c>
       <c r="C76" t="n">
-        <v>0.334795</v>
+        <v>0.107513</v>
       </c>
     </row>
     <row r="77">
@@ -1268,10 +1268,10 @@
         <v>76</v>
       </c>
       <c r="B77" t="n">
-        <v>0.439179</v>
+        <v>0.0324623</v>
       </c>
       <c r="C77" t="n">
-        <v>0.34269</v>
+        <v>0.112839</v>
       </c>
     </row>
     <row r="78">
@@ -1279,10 +1279,10 @@
         <v>77</v>
       </c>
       <c r="B78" t="n">
-        <v>0.439856</v>
+        <v>0.0314621</v>
       </c>
       <c r="C78" t="n">
-        <v>0.342768</v>
+        <v>0.10879</v>
       </c>
     </row>
     <row r="79">
@@ -1290,10 +1290,10 @@
         <v>78</v>
       </c>
       <c r="B79" t="n">
-        <v>0.4474</v>
+        <v>0.0315148</v>
       </c>
       <c r="C79" t="n">
-        <v>0.34972</v>
+        <v>0.111756</v>
       </c>
     </row>
     <row r="80">
@@ -1301,10 +1301,10 @@
         <v>79</v>
       </c>
       <c r="B80" t="n">
-        <v>0.468241</v>
+        <v>0.0302888</v>
       </c>
       <c r="C80" t="n">
-        <v>0.353391</v>
+        <v>0.144872</v>
       </c>
     </row>
     <row r="81">
@@ -1312,10 +1312,10 @@
         <v>80</v>
       </c>
       <c r="B81" t="n">
-        <v>0.456329</v>
+        <v>0.032548</v>
       </c>
       <c r="C81" t="n">
-        <v>0.356124</v>
+        <v>0.114621</v>
       </c>
     </row>
     <row r="82">
@@ -1323,10 +1323,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="n">
-        <v>0.4718</v>
+        <v>0.0298351</v>
       </c>
       <c r="C82" t="n">
-        <v>0.359115</v>
+        <v>0.111347</v>
       </c>
     </row>
     <row r="83">
@@ -1334,10 +1334,10 @@
         <v>82</v>
       </c>
       <c r="B83" t="n">
-        <v>0.470814</v>
+        <v>0.029173</v>
       </c>
       <c r="C83" t="n">
-        <v>0.363022</v>
+        <v>0.110588</v>
       </c>
     </row>
     <row r="84">
@@ -1345,10 +1345,10 @@
         <v>83</v>
       </c>
       <c r="B84" t="n">
-        <v>0.479035</v>
+        <v>0.0285799</v>
       </c>
       <c r="C84" t="n">
-        <v>0.368505</v>
+        <v>0.111092</v>
       </c>
     </row>
     <row r="85">
@@ -1356,10 +1356,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="n">
-        <v>0.484553</v>
+        <v>0.0282174</v>
       </c>
       <c r="C85" t="n">
-        <v>0.379847</v>
+        <v>0.115505</v>
       </c>
     </row>
     <row r="86">
@@ -1367,10 +1367,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="n">
-        <v>0.49919</v>
+        <v>0.0280146</v>
       </c>
       <c r="C86" t="n">
-        <v>0.38382</v>
+        <v>0.111858</v>
       </c>
     </row>
     <row r="87">
@@ -1378,10 +1378,10 @@
         <v>86</v>
       </c>
       <c r="B87" t="n">
-        <v>0.4922</v>
+        <v>0.0271155</v>
       </c>
       <c r="C87" t="n">
-        <v>0.382048</v>
+        <v>0.113191</v>
       </c>
     </row>
     <row r="88">
@@ -1389,10 +1389,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="n">
-        <v>0.50001</v>
+        <v>0.026867</v>
       </c>
       <c r="C88" t="n">
-        <v>0.398146</v>
+        <v>0.113801</v>
       </c>
     </row>
     <row r="89">
@@ -1400,10 +1400,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="n">
-        <v>0.512366</v>
+        <v>0.0265065</v>
       </c>
       <c r="C89" t="n">
-        <v>0.391403</v>
+        <v>0.114367</v>
       </c>
     </row>
     <row r="90">
@@ -1411,10 +1411,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="n">
-        <v>0.519594</v>
+        <v>0.0254739</v>
       </c>
       <c r="C90" t="n">
-        <v>0.396589</v>
+        <v>0.114017</v>
       </c>
     </row>
     <row r="91">
@@ -1422,10 +1422,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="n">
-        <v>0.5161559999999999</v>
+        <v>0.0250202</v>
       </c>
       <c r="C91" t="n">
-        <v>0.399603</v>
+        <v>0.114645</v>
       </c>
     </row>
     <row r="92">
@@ -1433,10 +1433,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="n">
-        <v>0.527379</v>
+        <v>0.0243298</v>
       </c>
       <c r="C92" t="n">
-        <v>0.405939</v>
+        <v>0.119862</v>
       </c>
     </row>
     <row r="93">
@@ -1444,10 +1444,10 @@
         <v>92</v>
       </c>
       <c r="B93" t="n">
-        <v>0.533375</v>
+        <v>0.0243701</v>
       </c>
       <c r="C93" t="n">
-        <v>0.41496</v>
+        <v>0.116532</v>
       </c>
     </row>
     <row r="94">
@@ -1455,10 +1455,10 @@
         <v>93</v>
       </c>
       <c r="B94" t="n">
-        <v>0.540015</v>
+        <v>0.0242332</v>
       </c>
       <c r="C94" t="n">
-        <v>0.419884</v>
+        <v>0.116866</v>
       </c>
     </row>
     <row r="95">
@@ -1466,10 +1466,10 @@
         <v>94</v>
       </c>
       <c r="B95" t="n">
-        <v>0.539739</v>
+        <v>0.0231271</v>
       </c>
       <c r="C95" t="n">
-        <v>0.421826</v>
+        <v>0.125036</v>
       </c>
     </row>
     <row r="96">
@@ -1477,10 +1477,10 @@
         <v>95</v>
       </c>
       <c r="B96" t="n">
-        <v>0.5430199999999999</v>
+        <v>0.0224824</v>
       </c>
       <c r="C96" t="n">
-        <v>0.421194</v>
+        <v>0.117722</v>
       </c>
     </row>
     <row r="97">
@@ -1488,10 +1488,10 @@
         <v>96</v>
       </c>
       <c r="B97" t="n">
-        <v>0.552723</v>
+        <v>0.0219052</v>
       </c>
       <c r="C97" t="n">
-        <v>0.42929</v>
+        <v>0.122868</v>
       </c>
     </row>
     <row r="98">
@@ -1499,10 +1499,10 @@
         <v>97</v>
       </c>
       <c r="B98" t="n">
-        <v>0.559503</v>
+        <v>0.0219857</v>
       </c>
       <c r="C98" t="n">
-        <v>0.439805</v>
+        <v>0.118383</v>
       </c>
     </row>
     <row r="99">
@@ -1510,10 +1510,10 @@
         <v>98</v>
       </c>
       <c r="B99" t="n">
-        <v>0.571561</v>
+        <v>0.0213325</v>
       </c>
       <c r="C99" t="n">
-        <v>0.441591</v>
+        <v>0.120636</v>
       </c>
     </row>
     <row r="100">
@@ -1521,10 +1521,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="n">
-        <v>0.575744</v>
+        <v>0.0204447</v>
       </c>
       <c r="C100" t="n">
-        <v>0.450074</v>
+        <v>0.127449</v>
       </c>
     </row>
     <row r="101">
@@ -1532,10 +1532,10 @@
         <v>100</v>
       </c>
       <c r="B101" t="n">
-        <v>0.579616</v>
+        <v>0.0204218</v>
       </c>
       <c r="C101" t="n">
-        <v>0.450786</v>
+        <v>0.120909</v>
       </c>
     </row>
     <row r="102">
@@ -1543,10 +1543,10 @@
         <v>101</v>
       </c>
       <c r="B102" t="n">
-        <v>0.593345</v>
+        <v>0.0203905</v>
       </c>
       <c r="C102" t="n">
-        <v>0.449268</v>
+        <v>0.120248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>